<commit_message>
V4.0.1 Fix Fecha y IF tipo
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0 AAAA.xlsx
+++ b/Archivo para hacer Facturas 3.0 AAAA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Facturador Multiusuario_20221202\Facturador Multiusuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Facturador-Multiusuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F30FFE-8CB9-41E7-BBC7-634A5A15425A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6171EB24-79D1-4AD0-B42E-04471F520F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
   <si>
     <t>Fecha</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Aux unidades</t>
-  </si>
-  <si>
-    <t>11/11/2022</t>
   </si>
   <si>
     <t>Factura A</t>
@@ -907,7 +904,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -959,7 +956,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1166,7 +1163,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,32 +1297,32 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>34</v>
+      <c r="A2" s="8">
+        <v>44992</v>
       </c>
       <c r="B2" s="9" t="str">
         <f>TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/yyyy")</f>
-        <v>01/10/yyyy</v>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C2" s="9" t="str">
-        <f>TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" ref="C2:C17" si="0">TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
+        <v>28/02/2023</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f>TEXT(A2+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" ref="D2:D17" si="1">TEXT(A2+14,"dd/mm/aaaa")</f>
+        <v>21/03/2023</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>9</v>
@@ -1334,11 +1331,11 @@
         <v>33610006189</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B2,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M2" s="4">
         <v>5.04</v>
@@ -1350,30 +1347,30 @@
         <v>44628.1</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
       <c r="T2" s="13"/>
       <c r="U2" s="1" t="str">
-        <f t="shared" ref="U2" si="0">TEXT(R2,"00000")</f>
+        <f t="shared" ref="U2" si="2">TEXT(R2,"00000")</f>
         <v>00000</v>
       </c>
       <c r="V2" s="1" t="str">
-        <f t="shared" ref="V2" si="1">TEXT(S2,"00000000")</f>
+        <f t="shared" ref="V2" si="3">TEXT(S2,"00000000")</f>
         <v>00000000</v>
       </c>
       <c r="W2" s="1" t="str">
-        <f>TEXT(T2,"DD/MM/aaaa")</f>
+        <f t="shared" ref="W2:W17" si="4">TEXT(T2,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
       <c r="X2" s="14">
-        <f t="shared" ref="X2" si="2">ROUND(O2*P2,2)</f>
+        <f t="shared" ref="X2" si="5">ROUND(O2*P2,2)</f>
         <v>9371.9</v>
       </c>
       <c r="Y2" s="14">
-        <f t="shared" ref="Y2" si="3">O2+X2</f>
+        <f t="shared" ref="Y2" si="6">O2+X2</f>
         <v>54000</v>
       </c>
       <c r="Z2" s="10" t="str">
@@ -1386,7 +1383,7 @@
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1">
-        <f t="shared" ref="AC2" si="4">ROW(K2)</f>
+        <f t="shared" ref="AC2" si="7">ROW(K2)</f>
         <v>2</v>
       </c>
       <c r="AD2" s="1" t="str">
@@ -1394,45 +1391,45 @@
         <v>33610006189-1</v>
       </c>
       <c r="AF2" s="15">
-        <f t="shared" ref="AF2" si="5">CEILING(N2*M2*(1+P2),500)</f>
+        <f t="shared" ref="AF2" si="8">CEILING(N2*M2*(1+P2),500)</f>
         <v>54000</v>
       </c>
       <c r="AG2" s="15">
-        <f t="shared" ref="AG2" si="6">ROUND((AF2/(1+P2)),2)</f>
+        <f t="shared" ref="AG2" si="9">ROUND((AF2/(1+P2)),2)</f>
         <v>44628.1</v>
       </c>
       <c r="AH2" s="16">
-        <f t="shared" ref="AH2" si="7">ROUND(AG2/N2,4)</f>
+        <f t="shared" ref="AH2" si="10">ROUND(AG2/N2,4)</f>
         <v>5.0419</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>34</v>
+      <c r="A3" s="8">
+        <v>44992</v>
       </c>
       <c r="B3" s="9" t="str">
-        <f t="shared" ref="B3:B17" si="8">TEXT(DATE(YEAR(C3),MONTH(C3),1),"dd/mm/yyyy")</f>
-        <v>01/10/yyyy</v>
+        <f t="shared" ref="B3:B17" si="11">TEXT(DATE(YEAR(C3),MONTH(C3),1),"dd/mm/yyyy")</f>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C3" s="9" t="str">
-        <f>TEXT(EOMONTH(A3,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f>TEXT(A3+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>9</v>
@@ -1441,10 +1438,10 @@
         <v>33610006189</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M3" s="4">
         <v>5.04</v>
@@ -1456,43 +1453,43 @@
         <v>44628.1</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="13"/>
       <c r="U3" s="1" t="str">
-        <f t="shared" ref="U3:U17" si="9">TEXT(R3,"00000")</f>
+        <f t="shared" ref="U3:U17" si="12">TEXT(R3,"00000")</f>
         <v>00000</v>
       </c>
       <c r="V3" s="1" t="str">
-        <f t="shared" ref="V3:V17" si="10">TEXT(S3,"00000000")</f>
+        <f t="shared" ref="V3:V17" si="13">TEXT(S3,"00000000")</f>
         <v>00000000</v>
       </c>
       <c r="W3" s="1" t="str">
-        <f>TEXT(T3,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X3" s="14">
-        <f t="shared" ref="X3:X17" si="11">ROUND(O3*P3,2)</f>
+        <f t="shared" ref="X3:X17" si="14">ROUND(O3*P3,2)</f>
         <v>9371.9</v>
       </c>
       <c r="Y3" s="14">
-        <f t="shared" ref="Y3:Y17" si="12">O3+X3</f>
+        <f t="shared" ref="Y3:Y17" si="15">O3+X3</f>
         <v>54000</v>
       </c>
       <c r="Z3" s="10" t="str">
-        <f t="shared" ref="Z3:Z17" si="13">IF(F3="Factura A",SUBSTITUTE(TEXT(O3,"0.00"),",","."),SUBSTITUTE(TEXT(Y3,"0.00"),",","."))</f>
+        <f t="shared" ref="Z3:Z17" si="16">IF(F3="Factura A",SUBSTITUTE(TEXT(O3,"0.00"),",","."),SUBSTITUTE(TEXT(Y3,"0.00"),",","."))</f>
         <v>44.628</v>
       </c>
       <c r="AA3" s="10" t="str">
-        <f t="shared" ref="AA3:AA17" si="14">SUBSTITUTE(TEXT(ROUNDUP(Y3,0)-Y3,"0.00"),",",".")</f>
+        <f t="shared" ref="AA3:AA17" si="17">SUBSTITUTE(TEXT(ROUNDUP(Y3,0)-Y3,"0.00"),",",".")</f>
         <v>000</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1">
-        <f t="shared" ref="AC3:AC17" si="15">ROW(K3)</f>
+        <f t="shared" ref="AC3:AC17" si="18">ROW(K3)</f>
         <v>3</v>
       </c>
       <c r="AD3" s="1" t="str">
@@ -1500,45 +1497,45 @@
         <v>33610006189-2</v>
       </c>
       <c r="AF3" s="15">
-        <f t="shared" ref="AF3:AF17" si="16">CEILING(N3*M3*(1+P3),500)</f>
+        <f t="shared" ref="AF3:AF17" si="19">CEILING(N3*M3*(1+P3),500)</f>
         <v>54000</v>
       </c>
       <c r="AG3" s="15">
-        <f t="shared" ref="AG3:AG17" si="17">ROUND((AF3/(1+P3)),2)</f>
+        <f t="shared" ref="AG3:AG17" si="20">ROUND((AF3/(1+P3)),2)</f>
         <v>44628.1</v>
       </c>
       <c r="AH3" s="16">
-        <f t="shared" ref="AH3:AH17" si="18">ROUND(AG3/N3,4)</f>
+        <f t="shared" ref="AH3:AH17" si="21">ROUND(AG3/N3,4)</f>
         <v>5.0419</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>34</v>
+      <c r="A4" s="8">
+        <v>44992</v>
       </c>
       <c r="B4" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f>TEXT(EOMONTH(A4,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f>TEXT(A4+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>9</v>
@@ -1547,11 +1544,11 @@
         <v>30610252334</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M4" s="4">
         <v>10.039999999999999</v>
@@ -1563,43 +1560,43 @@
         <v>88842.97</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
       <c r="T4" s="13"/>
       <c r="U4" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V4" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W4" s="1" t="str">
-        <f>TEXT(T4,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X4" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>18657.02</v>
       </c>
       <c r="Y4" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>107499.99</v>
       </c>
       <c r="Z4" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>88.843</v>
       </c>
       <c r="AA4" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="AD4" s="1" t="str">
@@ -1607,45 +1604,45 @@
         <v>30610252334-1</v>
       </c>
       <c r="AF4" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>108000</v>
       </c>
       <c r="AG4" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>89256.2</v>
       </c>
       <c r="AH4" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>10.0837</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>34</v>
+      <c r="A5" s="8">
+        <v>44992</v>
       </c>
       <c r="B5" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C5" s="9" t="str">
-        <f>TEXT(EOMONTH(A5,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D5" s="9" t="str">
-        <f>TEXT(A5+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>9</v>
@@ -1654,10 +1651,10 @@
         <v>30684125792</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="M5" s="4">
         <v>7</v>
@@ -1669,51 +1666,51 @@
         <v>61983.47</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="T5" s="13">
         <v>44816</v>
       </c>
       <c r="U5" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00002</v>
       </c>
       <c r="V5" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000150</v>
       </c>
       <c r="W5" s="1" t="str">
-        <f>TEXT(T5,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>12/09/2022</v>
       </c>
       <c r="X5" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>13016.53</v>
       </c>
       <c r="Y5" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>75000</v>
       </c>
       <c r="Z5" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>75.000</v>
       </c>
       <c r="AA5" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="AD5" s="1" t="str">
@@ -1721,45 +1718,45 @@
         <v>30684125792-1</v>
       </c>
       <c r="AF5" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>75000</v>
       </c>
       <c r="AG5" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>61983.47</v>
       </c>
       <c r="AH5" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7.0026000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>34</v>
+      <c r="A6" s="8">
+        <v>44992</v>
       </c>
       <c r="B6" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C6" s="9" t="str">
-        <f>TEXT(EOMONTH(A6,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D6" s="9" t="str">
-        <f>TEXT(A6+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>9</v>
@@ -1768,10 +1765,10 @@
         <v>30684125792</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="M6" s="4">
         <v>7</v>
@@ -1783,51 +1780,51 @@
         <v>61983.47</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="T6" s="13">
         <v>44816</v>
       </c>
       <c r="U6" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00002</v>
       </c>
       <c r="V6" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000151</v>
       </c>
       <c r="W6" s="1" t="str">
-        <f>TEXT(T6,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>12/09/2022</v>
       </c>
       <c r="X6" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>13016.53</v>
       </c>
       <c r="Y6" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>75000</v>
       </c>
       <c r="Z6" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>75.000</v>
       </c>
       <c r="AA6" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AD6" s="1" t="str">
@@ -1835,45 +1832,45 @@
         <v>30684125792-2</v>
       </c>
       <c r="AF6" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>75000</v>
       </c>
       <c r="AG6" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>61983.47</v>
       </c>
       <c r="AH6" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7.0026000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>34</v>
+      <c r="A7" s="8">
+        <v>44992</v>
       </c>
       <c r="B7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C7" s="9" t="str">
-        <f>TEXT(EOMONTH(A7,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D7" s="9" t="str">
-        <f>TEXT(A7+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>9</v>
@@ -1882,11 +1879,11 @@
         <v>30525733870</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B7,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M7" s="4">
         <v>8.0299999999999994</v>
@@ -1898,43 +1895,43 @@
         <v>71074.38</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="13"/>
       <c r="U7" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V7" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W7" s="1" t="str">
-        <f>TEXT(T7,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X7" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>14925.62</v>
       </c>
       <c r="Y7" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>86000</v>
       </c>
       <c r="Z7" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>71.074</v>
       </c>
       <c r="AA7" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
       <c r="AD7" s="1" t="str">
@@ -1942,45 +1939,45 @@
         <v>30525733870-1</v>
       </c>
       <c r="AF7" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>86500</v>
       </c>
       <c r="AG7" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>71487.600000000006</v>
       </c>
       <c r="AH7" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>8.0762999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>34</v>
+      <c r="A8" s="8">
+        <v>44992</v>
       </c>
       <c r="B8" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C8" s="9" t="str">
-        <f>TEXT(EOMONTH(A8,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D8" s="9" t="str">
-        <f>TEXT(A8+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>9</v>
@@ -1989,11 +1986,11 @@
         <v>30710964277</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M8" s="4">
         <v>9.01</v>
@@ -2005,43 +2002,43 @@
         <v>79752.070000000007</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
       <c r="T8" s="13"/>
       <c r="U8" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V8" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W8" s="1" t="str">
-        <f>TEXT(T8,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X8" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>16747.93</v>
       </c>
       <c r="Y8" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>96500</v>
       </c>
       <c r="Z8" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>79.752</v>
       </c>
       <c r="AA8" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="AD8" s="1" t="str">
@@ -2049,45 +2046,45 @@
         <v>30710964277-1</v>
       </c>
       <c r="AF8" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>97000</v>
       </c>
       <c r="AG8" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>80165.289999999994</v>
       </c>
       <c r="AH8" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>9.0566999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>34</v>
+      <c r="A9" s="8">
+        <v>44992</v>
       </c>
       <c r="B9" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C9" s="9" t="str">
-        <f>TEXT(EOMONTH(A9,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D9" s="9" t="str">
-        <f>TEXT(A9+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>9</v>
@@ -2096,11 +2093,11 @@
         <v>33615420269</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B9,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M9" s="4">
         <v>10.039999999999999</v>
@@ -2112,43 +2109,43 @@
         <v>88842.97</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
       <c r="T9" s="13"/>
       <c r="U9" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V9" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W9" s="1" t="str">
-        <f>TEXT(T9,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X9" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>18657.02</v>
       </c>
       <c r="Y9" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>107499.99</v>
       </c>
       <c r="Z9" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>88.843</v>
       </c>
       <c r="AA9" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="AD9" s="1" t="str">
@@ -2156,45 +2153,45 @@
         <v>33615420269-1</v>
       </c>
       <c r="AF9" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>108000</v>
       </c>
       <c r="AG9" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>89256.2</v>
       </c>
       <c r="AH9" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>10.0837</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>34</v>
+      <c r="A10" s="8">
+        <v>44992</v>
       </c>
       <c r="B10" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C10" s="9" t="str">
-        <f>TEXT(EOMONTH(A10,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D10" s="9" t="str">
-        <f>TEXT(A10+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>9</v>
@@ -2203,10 +2200,10 @@
         <v>30525390086</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="M10" s="4">
         <v>9.01</v>
@@ -2218,43 +2215,43 @@
         <v>79752.070000000007</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="13"/>
       <c r="U10" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V10" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W10" s="1" t="str">
-        <f>TEXT(T10,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X10" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>16747.93</v>
       </c>
       <c r="Y10" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>96500</v>
       </c>
       <c r="Z10" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>79.752</v>
       </c>
       <c r="AA10" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="AD10" s="1" t="str">
@@ -2262,45 +2259,45 @@
         <v>30525390086-1</v>
       </c>
       <c r="AF10" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>97000</v>
       </c>
       <c r="AG10" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>80165.289999999994</v>
       </c>
       <c r="AH10" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>9.0566999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>34</v>
+      <c r="A11" s="8">
+        <v>44992</v>
       </c>
       <c r="B11" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C11" s="9" t="str">
-        <f>TEXT(EOMONTH(A11,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D11" s="9" t="str">
-        <f>TEXT(A11+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>9</v>
@@ -2309,11 +2306,11 @@
         <v>20374730429</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L11" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B11,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M11" s="4">
         <v>1.03</v>
@@ -2325,43 +2322,43 @@
         <v>9090.91</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="13"/>
       <c r="U11" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V11" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W11" s="1" t="str">
-        <f>TEXT(T11,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X11" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y11" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z11" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>9.091</v>
       </c>
       <c r="AA11" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="AD11" s="1" t="str">
@@ -2369,45 +2366,45 @@
         <v>20374730429-1</v>
       </c>
       <c r="AF11" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG11" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH11" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>34</v>
+      <c r="A12" s="8">
+        <v>44992</v>
       </c>
       <c r="B12" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C12" s="9" t="str">
-        <f>TEXT(EOMONTH(A12,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D12" s="9" t="str">
-        <f>TEXT(A12+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>9</v>
@@ -2416,11 +2413,11 @@
         <v>20147130202</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L12" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B12,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M12" s="4">
         <v>1.03</v>
@@ -2432,43 +2429,43 @@
         <v>9090.91</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
       <c r="T12" s="13"/>
       <c r="U12" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V12" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W12" s="1" t="str">
-        <f>TEXT(T12,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X12" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y12" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z12" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>9.091</v>
       </c>
       <c r="AA12" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="AD12" s="1" t="str">
@@ -2476,45 +2473,45 @@
         <v>20147130202-1</v>
       </c>
       <c r="AF12" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG12" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH12" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>34</v>
+      <c r="A13" s="8">
+        <v>44992</v>
       </c>
       <c r="B13" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C13" s="9" t="str">
-        <f>TEXT(EOMONTH(A13,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D13" s="9" t="str">
-        <f>TEXT(A13+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>9</v>
@@ -2523,11 +2520,11 @@
         <v>30707354719</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L13" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B13,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M13" s="4">
         <v>1.03</v>
@@ -2539,43 +2536,43 @@
         <v>9090.91</v>
       </c>
       <c r="P13" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
       <c r="T13" s="13"/>
       <c r="U13" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V13" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W13" s="1" t="str">
-        <f>TEXT(T13,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X13" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y13" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z13" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>11.000</v>
       </c>
       <c r="AA13" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="AD13" s="1" t="str">
@@ -2583,58 +2580,58 @@
         <v>30707354719-1</v>
       </c>
       <c r="AF13" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG13" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH13" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>34</v>
+      <c r="A14" s="8">
+        <v>44992</v>
       </c>
       <c r="B14" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C14" s="9" t="str">
-        <f>TEXT(EOMONTH(A14,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D14" s="9" t="str">
-        <f>TEXT(A14+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="J14" s="2">
         <v>37473042</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L14" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B14,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M14" s="4">
         <v>1.03</v>
@@ -2646,43 +2643,43 @@
         <v>9090.91</v>
       </c>
       <c r="P14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="13"/>
       <c r="U14" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V14" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W14" s="1" t="str">
-        <f>TEXT(T14,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X14" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y14" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z14" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>11.000</v>
       </c>
       <c r="AA14" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="AD14" s="1" t="str">
@@ -2690,45 +2687,45 @@
         <v>37473042-1</v>
       </c>
       <c r="AF14" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG14" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH14" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>34</v>
+      <c r="A15" s="8">
+        <v>44992</v>
       </c>
       <c r="B15" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C15" s="9" t="str">
-        <f>TEXT(EOMONTH(A15,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D15" s="9" t="str">
-        <f>TEXT(A15+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>9</v>
@@ -2737,10 +2734,10 @@
         <v>30707354719</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M15" s="4">
         <v>1.03</v>
@@ -2752,51 +2749,51 @@
         <v>9090.91</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q15" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S15" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T15" s="13">
         <v>44816</v>
       </c>
       <c r="U15" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00002</v>
       </c>
       <c r="V15" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000152</v>
       </c>
       <c r="W15" s="1" t="str">
-        <f>TEXT(T15,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>12/09/2022</v>
       </c>
       <c r="X15" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y15" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z15" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>11.000</v>
       </c>
       <c r="AA15" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="AD15" s="1" t="str">
@@ -2804,57 +2801,57 @@
         <v>30707354719-2</v>
       </c>
       <c r="AF15" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG15" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH15" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>34</v>
+      <c r="A16" s="8">
+        <v>44992</v>
       </c>
       <c r="B16" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C16" s="9" t="str">
-        <f>TEXT(EOMONTH(A16,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D16" s="9" t="str">
-        <f>TEXT(A16+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="J16" s="2">
         <v>37473042</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M16" s="4">
         <v>1.03</v>
@@ -2866,51 +2863,51 @@
         <v>9090.91</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S16" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="R16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="S16" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="T16" s="13">
         <v>44816</v>
       </c>
       <c r="U16" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00002</v>
       </c>
       <c r="V16" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000153</v>
       </c>
       <c r="W16" s="1" t="str">
-        <f>TEXT(T16,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>12/09/2022</v>
       </c>
       <c r="X16" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y16" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z16" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>11.000</v>
       </c>
       <c r="AA16" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="AD16" s="1" t="str">
@@ -2918,56 +2915,56 @@
         <v>37473042-2</v>
       </c>
       <c r="AF16" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG16" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH16" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>34</v>
+      <c r="A17" s="8">
+        <v>44992</v>
       </c>
       <c r="B17" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>01/10/yyyy</v>
+        <f t="shared" si="11"/>
+        <v>01/02/yyyy</v>
       </c>
       <c r="C17" s="9" t="str">
-        <f>TEXT(EOMONTH(A17,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D17" s="9" t="str">
-        <f>TEXT(A17+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="1"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L17" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B17,"mmmm"))</f>
-        <v>Honorarios 01/10/Yyyy</v>
+        <v>Honorarios 01/02/Yyyy</v>
       </c>
       <c r="M17" s="4">
         <v>1.03</v>
@@ -2979,43 +2976,43 @@
         <v>0</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
       <c r="T17" s="13"/>
       <c r="U17" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000</v>
       </c>
       <c r="V17" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
       <c r="W17" s="1" t="str">
-        <f>TEXT(T17,"DD/MM/aaaa")</f>
+        <f t="shared" si="4"/>
         <v>00/01/1900</v>
       </c>
       <c r="X17" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y17" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Z17" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>000</v>
       </c>
       <c r="AA17" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>17</v>
       </c>
       <c r="AD17" s="1" t="str">
@@ -3023,15 +3020,15 @@
         <v>-0</v>
       </c>
       <c r="AF17" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG17" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH17" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix #1:Update Excels to match bot
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0 AAAA.xlsx
+++ b/Archivo para hacer Facturas 3.0 AAAA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Facturador-Multiusuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D87973C-B38D-4F12-A77E-6A90A6FD7B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A242E0BA-9E99-4129-BD97-417636290D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Factura" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AD$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AP$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
   <si>
     <t>Fecha</t>
   </si>
@@ -249,6 +249,42 @@
   </si>
   <si>
     <t>MARTIN BUSTOS</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Anterior</t>
+  </si>
+  <si>
+    <t>Posterior</t>
+  </si>
+  <si>
+    <t>Derecha Tipo</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Remito R</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Unidades Facturador</t>
+  </si>
+  <si>
+    <t>Precio Facturador</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Mult Sup 500</t>
+  </si>
+  <si>
+    <t>AUX unidades mult</t>
   </si>
 </sst>
 </file>
@@ -257,7 +293,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.000000_ ;_ * \-#,##0.000000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -600,7 +636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -730,6 +766,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -776,7 +825,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -791,11 +840,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="35" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1158,12 +1211,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH17"/>
+  <dimension ref="A1:AR17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,22 +1230,28 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
     <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="23" width="9.140625" customWidth="1"/>
-    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" customWidth="1"/>
-    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="9.140625" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="26" width="9.140625" customWidth="1"/>
+    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" customWidth="1"/>
+    <col min="32" max="32" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6" customWidth="1"/>
+    <col min="35" max="35" width="5.85546875" customWidth="1"/>
+    <col min="36" max="36" width="4" customWidth="1"/>
+    <col min="37" max="37" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1254,63 +1313,94 @@
         <v>19</v>
       </c>
       <c r="U1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AG1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AH1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AM1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AN1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AO1" s="17" t="s">
         <v>33</v>
       </c>
+      <c r="AP1" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ1" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR1" s="19" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B2" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f ca="1">TODAY()</f>
+        <v>45069</v>
+      </c>
+      <c r="B2" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C2" s="9" t="str">
-        <f t="shared" ref="C2:C17" si="0">TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A2,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f t="shared" ref="D2:D17" si="1">TEXT(A2+14,"dd/mm/aaaa")</f>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A2+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1319,7 +1409,7 @@
         <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>36</v>
@@ -1328,23 +1418,23 @@
         <v>9</v>
       </c>
       <c r="J2" s="3">
-        <v>33610006189</v>
+        <v>30525390086</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B2,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>53</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="M2" s="4">
-        <v>5.04</v>
-      </c>
-      <c r="N2" s="2">
-        <v>8851.52</v>
+        <v>7.003044</v>
+      </c>
+      <c r="N2" s="5">
+        <v>19000</v>
       </c>
       <c r="O2" s="5">
-        <v>44628.1</v>
+        <f>M2*N2</f>
+        <v>133057.83600000001</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>38</v>
@@ -1352,72 +1442,111 @@
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="1" t="str">
-        <f t="shared" ref="U2" si="2">TEXT(R2,"00000")</f>
+      <c r="T2" s="12"/>
+      <c r="U2" s="14">
+        <f>COUNTIFS($F$1:F2,F2,$K$1:K2,K2)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V2" s="18" t="str">
+        <f t="shared" ref="V2:V17" si="0">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
+        <v>7.003044</v>
+      </c>
+      <c r="W2" s="18" t="str">
+        <f>SUBSTITUTE(TEXT(N2,"0,00"),",",".")</f>
+        <v>19000.00</v>
+      </c>
+      <c r="X2" s="1" t="str">
+        <f t="shared" ref="X2:X17" si="1">TEXT(R2,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V2" s="1" t="str">
-        <f t="shared" ref="V2" si="3">TEXT(S2,"00000000")</f>
+      <c r="Y2" s="1" t="str">
+        <f t="shared" ref="Y2:Y17" si="2">TEXT(S2,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W2" s="1" t="str">
-        <f t="shared" ref="W2:W17" si="4">TEXT(T2,"DD/MM/aaaa")</f>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X2" s="14">
-        <f t="shared" ref="X2" si="5">ROUND(O2*P2,2)</f>
-        <v>9371.9</v>
-      </c>
-      <c r="Y2" s="14">
-        <f t="shared" ref="Y2" si="6">O2+X2</f>
-        <v>54000</v>
-      </c>
-      <c r="Z2" s="10" t="str">
-        <f t="shared" ref="Z2:Z16" si="7">IF(F2="Factura A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(Y2,"0,00"),",","."))</f>
-        <v>44628.10</v>
-      </c>
-      <c r="AA2" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(Y2,0)-Y2,"0,00"),",",".")</f>
-        <v>0.00</v>
-      </c>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1">
-        <f t="shared" ref="AC2" si="8">ROW(K2)</f>
+      <c r="Z2" s="1" t="str">
+        <f>TEXT(T2,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA2" s="13">
+        <f t="shared" ref="AA2:AA17" si="3">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
+        <v>27942.15</v>
+      </c>
+      <c r="AB2" s="13">
+        <f>IF(AJ2="A",ROUND(O2+AA2,2),ROUND(O2,2))</f>
+        <v>160999.99</v>
+      </c>
+      <c r="AC2" s="10" t="str">
+        <f t="shared" ref="AC2:AC17" si="4">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
+        <v>133057.84</v>
+      </c>
+      <c r="AD2" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AB2,0)-AB2,"0,00"),",",".")</f>
+        <v>0.01</v>
+      </c>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1">
+        <f t="shared" ref="AF2:AF17" si="5">ROW(K2)</f>
         <v>2</v>
       </c>
-      <c r="AD2" s="1" t="str">
+      <c r="AG2" s="15" t="str">
         <f>J2&amp;"-"&amp;COUNTIF($J$1:J2,J2)</f>
-        <v>33610006189-1</v>
-      </c>
-      <c r="AF2" s="15">
-        <f t="shared" ref="AF2" si="9">CEILING(N2*M2*(1+P2),500)</f>
-        <v>54000</v>
-      </c>
-      <c r="AG2" s="15">
-        <f t="shared" ref="AG2" si="10">ROUND((AF2/(1+P2)),2)</f>
-        <v>44628.1</v>
-      </c>
-      <c r="AH2" s="16">
-        <f t="shared" ref="AH2" si="11">ROUND(AG2/N2,4)</f>
-        <v>5.0419</v>
-      </c>
+        <v>30525390086-1</v>
+      </c>
+      <c r="AH2" s="1">
+        <f t="shared" ref="AH2:AH17" si="6">IF(K1=K2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1">
+        <f t="shared" ref="AI2:AI17" si="7">IF(K2=K3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <f t="shared" ref="AJ2:AJ17" si="8">RIGHT(F2)</f>
+        <v>A</v>
+      </c>
+      <c r="AK2" s="1">
+        <f>IF(LEFT(F2,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="13">
+        <f>IF(RIGHT(F2,1)="A",ROUND(N2*M2*(1+P2),2),AB2)</f>
+        <v>160999.98000000001</v>
+      </c>
+      <c r="AN2" s="13">
+        <f t="shared" ref="AN2:AN17" si="9">ROUND((AM2/(1+P2)),2)</f>
+        <v>133057.82999999999</v>
+      </c>
+      <c r="AO2" s="20">
+        <f t="shared" ref="AO2:AO17" si="10">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
+        <v>7.003044</v>
+      </c>
+      <c r="AP2" s="13">
+        <f t="shared" ref="AP2:AP17" si="11">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
+        <v>161000</v>
+      </c>
+      <c r="AQ2" s="20">
+        <f>IF(AJ2="A",ROUND(AN2/N2,6),AP2/N2)</f>
+        <v>7.003044</v>
+      </c>
+      <c r="AR2" s="2"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B3" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C3),MONTH(C3),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ref="A3:A17" ca="1" si="12">TODAY()</f>
+        <v>45069</v>
+      </c>
+      <c r="B3" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C3),MONTH(C3),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C3" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A3,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A3+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1435,22 +1564,24 @@
         <v>9</v>
       </c>
       <c r="J3" s="3">
-        <v>33610006189</v>
+        <v>30525733870</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="L3" s="1" t="e">
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="M3" s="4">
-        <v>5.04</v>
-      </c>
-      <c r="N3" s="2">
-        <v>8851.52</v>
+        <v>8.0252280000000003</v>
+      </c>
+      <c r="N3" s="5">
+        <v>19000</v>
       </c>
       <c r="O3" s="5">
-        <v>44628.1</v>
+        <f t="shared" ref="O3:O17" si="13">M3*N3</f>
+        <v>152479.33199999999</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>38</v>
@@ -1458,72 +1589,111 @@
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="1" t="str">
-        <f t="shared" ref="U3:U17" si="12">TEXT(R3,"00000")</f>
+      <c r="T3" s="12"/>
+      <c r="U3" s="14">
+        <f>COUNTIFS($F$1:F3,F3,$K$1:K3,K3)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V3" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>8.025228</v>
+      </c>
+      <c r="W3" s="18" t="str">
+        <f t="shared" ref="W3:W17" si="14">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
+        <v>19000.00</v>
+      </c>
+      <c r="X3" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V3" s="1" t="str">
-        <f t="shared" ref="V3:V17" si="13">TEXT(S3,"00000000")</f>
+      <c r="Y3" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W3" s="1" t="str">
+      <c r="Z3" s="1" t="str">
+        <f>TEXT(T3,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA3" s="13">
+        <f t="shared" si="3"/>
+        <v>32020.66</v>
+      </c>
+      <c r="AB3" s="13">
+        <f t="shared" ref="AB3:AB17" si="15">IF(AJ3="A",ROUND(O3+AA3,2),ROUND(O3,2))</f>
+        <v>184499.99</v>
+      </c>
+      <c r="AC3" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X3" s="14">
-        <f t="shared" ref="X3:X17" si="14">ROUND(O3*P3,2)</f>
-        <v>9371.9</v>
-      </c>
-      <c r="Y3" s="14">
-        <f t="shared" ref="Y3:Y17" si="15">O3+X3</f>
-        <v>54000</v>
-      </c>
-      <c r="Z3" s="10" t="str">
+        <v>152479.33</v>
+      </c>
+      <c r="AD3" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AB3,0)-AB3,"0,00"),",",".")</f>
+        <v>0.01</v>
+      </c>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="AG3" s="15" t="str">
+        <f>J3&amp;"-"&amp;COUNTIF($J$1:J3,J3)</f>
+        <v>30525733870-1</v>
+      </c>
+      <c r="AH3" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI3" s="1">
         <f t="shared" si="7"/>
-        <v>44628.10</v>
-      </c>
-      <c r="AA3" s="10" t="str">
-        <f t="shared" ref="AA3:AA17" si="16">SUBSTITUTE(TEXT(ROUNDUP(Y3,0)-Y3,"0,00"),",",".")</f>
-        <v>0.00</v>
-      </c>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1">
-        <f t="shared" ref="AC3:AC17" si="17">ROW(K3)</f>
-        <v>3</v>
-      </c>
-      <c r="AD3" s="1" t="str">
-        <f>J3&amp;"-"&amp;COUNTIF($J$1:J3,J3)</f>
-        <v>33610006189-2</v>
-      </c>
-      <c r="AF3" s="15">
-        <f t="shared" ref="AF3:AF17" si="18">CEILING(N3*M3*(1+P3),500)</f>
-        <v>54000</v>
-      </c>
-      <c r="AG3" s="15">
-        <f t="shared" ref="AG3:AG17" si="19">ROUND((AF3/(1+P3)),2)</f>
-        <v>44628.1</v>
-      </c>
-      <c r="AH3" s="16">
-        <f t="shared" ref="AH3:AH17" si="20">ROUND(AG3/N3,4)</f>
-        <v>5.0419</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK3" s="1">
+        <f t="shared" ref="AK3:AK17" si="16">IF(LEFT(F3,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="13">
+        <f t="shared" ref="AM3:AM17" si="17">IF(RIGHT(F3,1)="A",ROUND(N3*M3*(1+P3),2),AB3)</f>
+        <v>184499.99</v>
+      </c>
+      <c r="AN3" s="13">
+        <f t="shared" si="9"/>
+        <v>152479.32999999999</v>
+      </c>
+      <c r="AO3" s="20">
+        <f t="shared" si="10"/>
+        <v>8.0252280000000003</v>
+      </c>
+      <c r="AP3" s="13">
+        <f t="shared" si="11"/>
+        <v>184500</v>
+      </c>
+      <c r="AQ3" s="20">
+        <f t="shared" ref="AQ3:AQ17" si="18">IF(AJ3="A",ROUND(AN3/N3,6),AP3/N3)</f>
+        <v>8.0252280000000003</v>
+      </c>
+      <c r="AR3" s="2"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B4" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C4),MONTH(C4),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B4" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C4),MONTH(C4),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A4,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A4+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1546,18 +1716,19 @@
       <c r="K4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+      <c r="L4" s="1" t="e">
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="M4" s="4">
-        <v>10.039999999999999</v>
-      </c>
-      <c r="N4" s="2">
-        <v>8851.52</v>
+        <v>10.004348999999999</v>
+      </c>
+      <c r="N4" s="5">
+        <v>19000</v>
       </c>
       <c r="O4" s="5">
-        <v>88842.97</v>
+        <f t="shared" si="13"/>
+        <v>190082.63099999999</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>38</v>
@@ -1565,78 +1736,117 @@
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="14">
+        <f>COUNTIFS($F$1:F4,F4,$K$1:K4,K4)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V4" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10.004349</v>
+      </c>
+      <c r="W4" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V4" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y4" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W4" s="1" t="str">
+      <c r="Z4" s="1" t="str">
+        <f>TEXT(T4,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA4" s="13">
+        <f t="shared" si="3"/>
+        <v>39917.35</v>
+      </c>
+      <c r="AB4" s="13">
+        <f t="shared" si="15"/>
+        <v>229999.98</v>
+      </c>
+      <c r="AC4" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X4" s="14">
-        <f t="shared" si="14"/>
-        <v>18657.02</v>
-      </c>
-      <c r="Y4" s="14">
-        <f t="shared" si="15"/>
-        <v>107499.99</v>
-      </c>
-      <c r="Z4" s="10" t="str">
-        <f t="shared" si="7"/>
-        <v>88842.97</v>
-      </c>
-      <c r="AA4" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.01</v>
-      </c>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1">
-        <f t="shared" si="17"/>
+        <v>190082.63</v>
+      </c>
+      <c r="AD4" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AB4,0)-AB4,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AD4" s="1" t="str">
+      <c r="AG4" s="15" t="str">
         <f>J4&amp;"-"&amp;COUNTIF($J$1:J4,J4)</f>
         <v>30610252334-1</v>
       </c>
-      <c r="AF4" s="15">
+      <c r="AH4" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI4" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK4" s="1">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="13">
+        <f t="shared" si="17"/>
+        <v>229999.98</v>
+      </c>
+      <c r="AN4" s="13">
+        <f t="shared" si="9"/>
+        <v>190082.63</v>
+      </c>
+      <c r="AO4" s="20">
+        <f t="shared" si="10"/>
+        <v>10.004348999999999</v>
+      </c>
+      <c r="AP4" s="13">
+        <f t="shared" si="11"/>
+        <v>230000</v>
+      </c>
+      <c r="AQ4" s="20">
         <f t="shared" si="18"/>
-        <v>108000</v>
-      </c>
-      <c r="AG4" s="15">
-        <f t="shared" si="19"/>
-        <v>89256.2</v>
-      </c>
-      <c r="AH4" s="16">
-        <f t="shared" si="20"/>
-        <v>10.0837</v>
-      </c>
+        <v>10.004348999999999</v>
+      </c>
+      <c r="AR4" s="2"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B5" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C5),MONTH(C5),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B5" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C5),MONTH(C5),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C5" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A5,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D5" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A5+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>39</v>
@@ -1648,112 +1858,145 @@
         <v>9</v>
       </c>
       <c r="J5" s="3">
-        <v>30684125792</v>
+        <v>30710964277</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="L5" s="1" t="e">
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="M5" s="4">
-        <v>7</v>
-      </c>
-      <c r="N5" s="2">
-        <v>8851.52</v>
+        <v>9.0256629999999998</v>
+      </c>
+      <c r="N5" s="5">
+        <v>19000</v>
       </c>
       <c r="O5" s="5">
-        <v>61983.47</v>
+        <f t="shared" si="13"/>
+        <v>171487.59700000001</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="T5" s="13">
-        <v>44816</v>
-      </c>
-      <c r="U5" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>00002</v>
-      </c>
-      <c r="V5" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>00000150</v>
-      </c>
-      <c r="W5" s="1" t="str">
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="14">
+        <f>COUNTIFS($F$1:F5,F5,$K$1:K5,K5)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V5" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>9.025663</v>
+      </c>
+      <c r="W5" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z5" s="1" t="str">
+        <f>TEXT(T5,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA5" s="13">
+        <f t="shared" si="3"/>
+        <v>36012.400000000001</v>
+      </c>
+      <c r="AB5" s="13">
+        <f t="shared" si="15"/>
+        <v>207500</v>
+      </c>
+      <c r="AC5" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="X5" s="14">
-        <f t="shared" si="14"/>
-        <v>13016.53</v>
-      </c>
-      <c r="Y5" s="14">
-        <f t="shared" si="15"/>
-        <v>75000</v>
-      </c>
-      <c r="Z5" s="10" t="str">
+        <v>171487.60</v>
+      </c>
+      <c r="AD5" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AB5,0)-AB5,"0,00"),",",".")</f>
+        <v>0.00</v>
+      </c>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AG5" s="15" t="str">
+        <f>J5&amp;"-"&amp;COUNTIF($J$1:J5,J5)</f>
+        <v>30710964277-1</v>
+      </c>
+      <c r="AH5" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="1">
         <f t="shared" si="7"/>
-        <v>75000.00</v>
-      </c>
-      <c r="AA5" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK5" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="13">
         <f t="shared" si="17"/>
-        <v>5</v>
-      </c>
-      <c r="AD5" s="1" t="str">
-        <f>J5&amp;"-"&amp;COUNTIF($J$1:J5,J5)</f>
-        <v>30684125792-1</v>
-      </c>
-      <c r="AF5" s="15">
+        <v>207499.99</v>
+      </c>
+      <c r="AN5" s="13">
+        <f t="shared" si="9"/>
+        <v>171487.6</v>
+      </c>
+      <c r="AO5" s="20">
+        <f t="shared" si="10"/>
+        <v>9.0256629999999998</v>
+      </c>
+      <c r="AP5" s="13">
+        <f t="shared" si="11"/>
+        <v>207500</v>
+      </c>
+      <c r="AQ5" s="20">
         <f t="shared" si="18"/>
-        <v>75000</v>
-      </c>
-      <c r="AG5" s="15">
-        <f t="shared" si="19"/>
-        <v>61983.47</v>
-      </c>
-      <c r="AH5" s="16">
-        <f t="shared" si="20"/>
-        <v>7.0026000000000002</v>
-      </c>
+        <v>9.0256629999999998</v>
+      </c>
+      <c r="AR5" s="2"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B6" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C6),MONTH(C6),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B6" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C6),MONTH(C6),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A6,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D6" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A6+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>36</v>
@@ -1762,103 +2005,144 @@
         <v>9</v>
       </c>
       <c r="J6" s="3">
-        <v>30684125792</v>
+        <v>33610006189</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="L6" s="1" t="e">
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="M6" s="4">
-        <v>7</v>
-      </c>
-      <c r="N6" s="2">
-        <v>8851.52</v>
+        <v>5.0239229999999999</v>
+      </c>
+      <c r="N6" s="5">
+        <v>19000</v>
       </c>
       <c r="O6" s="5">
-        <v>61983.47</v>
+        <f t="shared" si="13"/>
+        <v>95454.536999999997</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>38</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="R6" s="11" t="s">
         <v>46</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="T6" s="13">
+        <v>77</v>
+      </c>
+      <c r="T6" s="12">
         <v>44816</v>
       </c>
-      <c r="U6" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="U6" s="14">
+        <f>COUNTIFS($F$1:F6,F6,$K$1:K6,K6)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V6" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>5.023923</v>
+      </c>
+      <c r="W6" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X6" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00002</v>
       </c>
-      <c r="V6" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>00000151</v>
-      </c>
-      <c r="W6" s="1" t="str">
+      <c r="Y6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000003</v>
+      </c>
+      <c r="Z6" s="1" t="str">
+        <f>TEXT(T6,"DD/MM/YYYY")</f>
+        <v>12/09/YYYY</v>
+      </c>
+      <c r="AA6" s="13">
+        <f t="shared" si="3"/>
+        <v>20045.45</v>
+      </c>
+      <c r="AB6" s="13">
+        <f t="shared" si="15"/>
+        <v>115499.99</v>
+      </c>
+      <c r="AC6" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="X6" s="14">
-        <f t="shared" si="14"/>
-        <v>13016.53</v>
-      </c>
-      <c r="Y6" s="14">
-        <f t="shared" si="15"/>
-        <v>75000</v>
-      </c>
-      <c r="Z6" s="10" t="str">
+        <v>95454.54</v>
+      </c>
+      <c r="AD6" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AB6,0)-AB6,"0,00"),",",".")</f>
+        <v>0.01</v>
+      </c>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AG6" s="15" t="str">
+        <f>J6&amp;"-"&amp;COUNTIF($J$1:J6,J6)</f>
+        <v>33610006189-1</v>
+      </c>
+      <c r="AH6" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1">
         <f t="shared" si="7"/>
-        <v>75000.00</v>
-      </c>
-      <c r="AA6" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK6" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="13">
         <f t="shared" si="17"/>
-        <v>6</v>
-      </c>
-      <c r="AD6" s="1" t="str">
-        <f>J6&amp;"-"&amp;COUNTIF($J$1:J6,J6)</f>
-        <v>30684125792-2</v>
-      </c>
-      <c r="AF6" s="15">
+        <v>115499.99</v>
+      </c>
+      <c r="AN6" s="13">
+        <f t="shared" si="9"/>
+        <v>95454.54</v>
+      </c>
+      <c r="AO6" s="20">
+        <f t="shared" si="10"/>
+        <v>5.0239229999999999</v>
+      </c>
+      <c r="AP6" s="13">
+        <f t="shared" si="11"/>
+        <v>115500</v>
+      </c>
+      <c r="AQ6" s="20">
         <f t="shared" si="18"/>
-        <v>75000</v>
-      </c>
-      <c r="AG6" s="15">
-        <f t="shared" si="19"/>
-        <v>61983.47</v>
-      </c>
-      <c r="AH6" s="16">
-        <f t="shared" si="20"/>
-        <v>7.0026000000000002</v>
-      </c>
+        <v>5.0239229999999999</v>
+      </c>
+      <c r="AR6" s="2"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B7" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C7),MONTH(C7),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B7" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C7),MONTH(C7),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A7,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D7" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A7+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -1876,23 +2160,23 @@
         <v>9</v>
       </c>
       <c r="J7" s="3">
-        <v>30525733870</v>
+        <v>33610006189</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B7,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>37</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="M7" s="4">
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="N7" s="2">
-        <v>8851.52</v>
+        <v>5.0021740000000001</v>
+      </c>
+      <c r="N7" s="5">
+        <v>19000</v>
       </c>
       <c r="O7" s="5">
-        <v>71074.38</v>
+        <f t="shared" si="13"/>
+        <v>95041.305999999997</v>
       </c>
       <c r="P7" s="11" t="s">
         <v>38</v>
@@ -1900,72 +2184,111 @@
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="14">
+        <f>COUNTIFS($F$1:F7,F7,$K$1:K7,K7)+1</f>
+        <v>3</v>
+      </c>
+      <c r="V7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>5.002174</v>
+      </c>
+      <c r="W7" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V7" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y7" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W7" s="1" t="str">
+      <c r="Z7" s="1" t="str">
+        <f>TEXT(T7,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA7" s="13">
+        <f t="shared" si="3"/>
+        <v>19958.669999999998</v>
+      </c>
+      <c r="AB7" s="13">
+        <f t="shared" si="15"/>
+        <v>114999.98</v>
+      </c>
+      <c r="AC7" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X7" s="14">
-        <f t="shared" si="14"/>
-        <v>14925.62</v>
-      </c>
-      <c r="Y7" s="14">
-        <f t="shared" si="15"/>
-        <v>86000</v>
-      </c>
-      <c r="Z7" s="10" t="str">
+        <v>95041.31</v>
+      </c>
+      <c r="AD7" s="10" t="str">
+        <f t="shared" ref="AD7:AD17" si="19">SUBSTITUTE(TEXT(ROUNDUP(AB7,0)-AB7,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="AG7" s="15" t="str">
+        <f>J7&amp;"-"&amp;COUNTIF($J$1:J7,J7)</f>
+        <v>33610006189-2</v>
+      </c>
+      <c r="AH7" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AI7" s="1">
         <f t="shared" si="7"/>
-        <v>71074.38</v>
-      </c>
-      <c r="AA7" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK7" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="13">
         <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="AD7" s="1" t="str">
-        <f>J7&amp;"-"&amp;COUNTIF($J$1:J7,J7)</f>
-        <v>30525733870-1</v>
-      </c>
-      <c r="AF7" s="15">
+        <v>114999.98</v>
+      </c>
+      <c r="AN7" s="13">
+        <f t="shared" si="9"/>
+        <v>95041.31</v>
+      </c>
+      <c r="AO7" s="20">
+        <f t="shared" si="10"/>
+        <v>5.0021740000000001</v>
+      </c>
+      <c r="AP7" s="13">
+        <f t="shared" si="11"/>
+        <v>115000</v>
+      </c>
+      <c r="AQ7" s="20">
         <f t="shared" si="18"/>
-        <v>86500</v>
-      </c>
-      <c r="AG7" s="15">
-        <f t="shared" si="19"/>
-        <v>71487.600000000006</v>
-      </c>
-      <c r="AH7" s="16">
-        <f t="shared" si="20"/>
-        <v>8.0762999999999998</v>
-      </c>
+        <v>5.0021740000000001</v>
+      </c>
+      <c r="AR7" s="2"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B8" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C8),MONTH(C8),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B8" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C8),MONTH(C8),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A8,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D8" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A8+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -1983,23 +2306,24 @@
         <v>9</v>
       </c>
       <c r="J8" s="3">
-        <v>30710964277</v>
+        <v>33615420269</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>52</v>
+      </c>
+      <c r="L8" s="1" t="e">
+        <f t="shared" ref="L8:L13" ca="1" si="20">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="M8" s="4">
-        <v>9.01</v>
-      </c>
-      <c r="N8" s="2">
-        <v>8851.52</v>
+        <v>10.004348999999999</v>
+      </c>
+      <c r="N8" s="5">
+        <v>19000</v>
       </c>
       <c r="O8" s="5">
-        <v>79752.070000000007</v>
+        <f t="shared" si="13"/>
+        <v>190082.63099999999</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>38</v>
@@ -2007,72 +2331,111 @@
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="14">
+        <f>COUNTIFS($F$1:F8,F8,$K$1:K8,K8)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10.004349</v>
+      </c>
+      <c r="W8" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V8" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y8" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W8" s="1" t="str">
+      <c r="Z8" s="1" t="str">
+        <f>TEXT(T8,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA8" s="13">
+        <f t="shared" si="3"/>
+        <v>39917.35</v>
+      </c>
+      <c r="AB8" s="13">
+        <f t="shared" si="15"/>
+        <v>229999.98</v>
+      </c>
+      <c r="AC8" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X8" s="14">
-        <f t="shared" si="14"/>
-        <v>16747.93</v>
-      </c>
-      <c r="Y8" s="14">
-        <f t="shared" si="15"/>
-        <v>96500</v>
-      </c>
-      <c r="Z8" s="10" t="str">
+        <v>190082.63</v>
+      </c>
+      <c r="AD8" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.02</v>
+      </c>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AG8" s="15" t="str">
+        <f>J8&amp;"-"&amp;COUNTIF($J$1:J8,J8)</f>
+        <v>33615420269-1</v>
+      </c>
+      <c r="AH8" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="1">
         <f t="shared" si="7"/>
-        <v>79752.07</v>
-      </c>
-      <c r="AA8" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK8" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="13">
         <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="AD8" s="1" t="str">
-        <f>J8&amp;"-"&amp;COUNTIF($J$1:J8,J8)</f>
-        <v>30710964277-1</v>
-      </c>
-      <c r="AF8" s="15">
+        <v>229999.98</v>
+      </c>
+      <c r="AN8" s="13">
+        <f t="shared" si="9"/>
+        <v>190082.63</v>
+      </c>
+      <c r="AO8" s="20">
+        <f t="shared" si="10"/>
+        <v>10.004348999999999</v>
+      </c>
+      <c r="AP8" s="13">
+        <f t="shared" si="11"/>
+        <v>230000</v>
+      </c>
+      <c r="AQ8" s="20">
         <f t="shared" si="18"/>
-        <v>97000</v>
-      </c>
-      <c r="AG8" s="15">
-        <f t="shared" si="19"/>
-        <v>80165.289999999994</v>
-      </c>
-      <c r="AH8" s="16">
-        <f t="shared" si="20"/>
-        <v>9.0566999999999993</v>
-      </c>
+        <v>10.004348999999999</v>
+      </c>
+      <c r="AR8" s="2"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B9" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C9),MONTH(C9),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B9" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C9),MONTH(C9),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A9,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D9" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A9+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2084,29 +2447,30 @@
         <v>39</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="3">
-        <v>33615420269</v>
+      <c r="J9" s="2">
+        <v>20147130202</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B9,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>57</v>
+      </c>
+      <c r="L9" s="1" t="e">
+        <f t="shared" ca="1" si="20"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M9" s="4">
-        <v>10.039999999999999</v>
-      </c>
-      <c r="N9" s="2">
-        <v>8851.52</v>
+        <v>1.0221830000000001</v>
+      </c>
+      <c r="N9" s="5">
+        <v>19000</v>
       </c>
       <c r="O9" s="5">
-        <v>88842.97</v>
+        <f t="shared" si="13"/>
+        <v>19421.477000000003</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>38</v>
@@ -2114,72 +2478,111 @@
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="14">
+        <f>COUNTIFS($F$1:F9,F9,$K$1:K9,K9)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.022183</v>
+      </c>
+      <c r="W9" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V9" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y9" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W9" s="1" t="str">
+      <c r="Z9" s="1" t="str">
+        <f>TEXT(T9,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA9" s="13">
+        <f t="shared" si="3"/>
+        <v>4078.51</v>
+      </c>
+      <c r="AB9" s="13">
+        <f t="shared" si="15"/>
+        <v>23499.99</v>
+      </c>
+      <c r="AC9" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X9" s="14">
-        <f t="shared" si="14"/>
-        <v>18657.02</v>
-      </c>
-      <c r="Y9" s="14">
-        <f t="shared" si="15"/>
-        <v>107499.99</v>
-      </c>
-      <c r="Z9" s="10" t="str">
+        <v>19421.48</v>
+      </c>
+      <c r="AD9" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.01</v>
+      </c>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="AG9" s="15" t="str">
+        <f>J9&amp;"-"&amp;COUNTIF($J$1:J9,J9)</f>
+        <v>20147130202-1</v>
+      </c>
+      <c r="AH9" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="1">
         <f t="shared" si="7"/>
-        <v>88842.97</v>
-      </c>
-      <c r="AA9" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK9" s="1">
         <f t="shared" si="16"/>
-        <v>0.01</v>
-      </c>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="13">
         <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="AD9" s="1" t="str">
-        <f>J9&amp;"-"&amp;COUNTIF($J$1:J9,J9)</f>
-        <v>33615420269-1</v>
-      </c>
-      <c r="AF9" s="15">
+        <v>23499.99</v>
+      </c>
+      <c r="AN9" s="13">
+        <f t="shared" si="9"/>
+        <v>19421.48</v>
+      </c>
+      <c r="AO9" s="20">
+        <f t="shared" si="10"/>
+        <v>1.0221830000000001</v>
+      </c>
+      <c r="AP9" s="13">
+        <f t="shared" si="11"/>
+        <v>23500</v>
+      </c>
+      <c r="AQ9" s="20">
         <f t="shared" si="18"/>
-        <v>108000</v>
-      </c>
-      <c r="AG9" s="15">
-        <f t="shared" si="19"/>
-        <v>89256.2</v>
-      </c>
-      <c r="AH9" s="16">
-        <f t="shared" si="20"/>
-        <v>10.0837</v>
-      </c>
+        <v>1.0221830000000001</v>
+      </c>
+      <c r="AR9" s="2"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B10" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C10),MONTH(C10),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B10" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C10),MONTH(C10),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A10,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D10" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A10+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2191,28 +2594,30 @@
         <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="3">
-        <v>30525390086</v>
+      <c r="J10" s="2">
+        <v>20374730429</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="L10" s="1" t="e">
+        <f t="shared" ca="1" si="20"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M10" s="4">
-        <v>9.01</v>
-      </c>
-      <c r="N10" s="2">
-        <v>8851.52</v>
+        <v>1.0439320000000001</v>
+      </c>
+      <c r="N10" s="5">
+        <v>19000</v>
       </c>
       <c r="O10" s="5">
-        <v>79752.070000000007</v>
+        <f t="shared" si="13"/>
+        <v>19834.708000000002</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>38</v>
@@ -2220,106 +2625,146 @@
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="14">
+        <f>COUNTIFS($F$1:F10,F10,$K$1:K10,K10)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.043932</v>
+      </c>
+      <c r="W10" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X10" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V10" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y10" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W10" s="1" t="str">
+      <c r="Z10" s="1" t="str">
+        <f>TEXT(T10,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA10" s="13">
+        <f t="shared" si="3"/>
+        <v>4165.29</v>
+      </c>
+      <c r="AB10" s="13">
+        <f t="shared" si="15"/>
+        <v>24000</v>
+      </c>
+      <c r="AC10" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X10" s="14">
-        <f t="shared" si="14"/>
-        <v>16747.93</v>
-      </c>
-      <c r="Y10" s="14">
-        <f t="shared" si="15"/>
-        <v>96500</v>
-      </c>
-      <c r="Z10" s="10" t="str">
+        <v>19834.71</v>
+      </c>
+      <c r="AD10" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.00</v>
+      </c>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AG10" s="15" t="str">
+        <f>J10&amp;"-"&amp;COUNTIF($J$1:J10,J10)</f>
+        <v>20374730429-1</v>
+      </c>
+      <c r="AH10" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI10" s="1">
         <f t="shared" si="7"/>
-        <v>79752.07</v>
-      </c>
-      <c r="AA10" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK10" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="13">
         <f t="shared" si="17"/>
-        <v>10</v>
-      </c>
-      <c r="AD10" s="1" t="str">
-        <f>J10&amp;"-"&amp;COUNTIF($J$1:J10,J10)</f>
-        <v>30525390086-1</v>
-      </c>
-      <c r="AF10" s="15">
+        <v>24000</v>
+      </c>
+      <c r="AN10" s="13">
+        <f t="shared" si="9"/>
+        <v>19834.71</v>
+      </c>
+      <c r="AO10" s="20">
+        <f t="shared" si="10"/>
+        <v>1.0439320000000001</v>
+      </c>
+      <c r="AP10" s="13">
+        <f t="shared" si="11"/>
+        <v>24000</v>
+      </c>
+      <c r="AQ10" s="20">
         <f t="shared" si="18"/>
-        <v>97000</v>
-      </c>
-      <c r="AG10" s="15">
-        <f t="shared" si="19"/>
-        <v>80165.289999999994</v>
-      </c>
-      <c r="AH10" s="16">
-        <f t="shared" si="20"/>
-        <v>9.0566999999999993</v>
-      </c>
+        <v>1.0439320000000001</v>
+      </c>
+      <c r="AR10" s="2"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B11" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C11),MONTH(C11),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B11" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C11),MONTH(C11),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A11,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D11" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A11+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="J11" s="2">
-        <v>20374730429</v>
+        <v>37473042</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B11,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+      <c r="L11" s="1" t="e">
+        <f t="shared" ca="1" si="20"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M11" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N11" s="2">
-        <v>8851.52</v>
+        <v>1.3</v>
+      </c>
+      <c r="N11" s="5">
+        <v>10000</v>
       </c>
       <c r="O11" s="5">
-        <v>9090.91</v>
+        <f t="shared" si="13"/>
+        <v>13000</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>38</v>
@@ -2327,106 +2772,146 @@
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="14">
+        <f>COUNTIFS($F$1:F11,F11,$K$1:K11,K11)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="W11" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>10000.00</v>
+      </c>
+      <c r="X11" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V11" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y11" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W11" s="1" t="str">
+      <c r="Z11" s="1" t="str">
+        <f>TEXT(T11,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA11" s="13">
+        <f t="shared" si="3"/>
+        <v>2256.1999999999998</v>
+      </c>
+      <c r="AB11" s="13">
+        <f t="shared" si="15"/>
+        <v>13000</v>
+      </c>
+      <c r="AC11" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X11" s="14">
-        <f t="shared" si="14"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y11" s="14">
-        <f t="shared" si="15"/>
-        <v>11000</v>
-      </c>
-      <c r="Z11" s="10" t="str">
+        <v>13000.00</v>
+      </c>
+      <c r="AD11" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.00</v>
+      </c>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="AG11" s="15" t="str">
+        <f>J11&amp;"-"&amp;COUNTIF($J$1:J11,J11)</f>
+        <v>37473042-1</v>
+      </c>
+      <c r="AH11" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AI11" s="1">
         <f t="shared" si="7"/>
-        <v>9090.91</v>
-      </c>
-      <c r="AA11" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>B</v>
+      </c>
+      <c r="AK11" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="13">
         <f t="shared" si="17"/>
-        <v>11</v>
-      </c>
-      <c r="AD11" s="1" t="str">
-        <f>J11&amp;"-"&amp;COUNTIF($J$1:J11,J11)</f>
-        <v>20374730429-1</v>
-      </c>
-      <c r="AF11" s="15">
+        <v>13000</v>
+      </c>
+      <c r="AN11" s="13">
+        <f t="shared" si="9"/>
+        <v>10743.8</v>
+      </c>
+      <c r="AO11" s="20">
+        <f t="shared" si="10"/>
+        <v>1.3</v>
+      </c>
+      <c r="AP11" s="13">
+        <f t="shared" si="11"/>
+        <v>13000</v>
+      </c>
+      <c r="AQ11" s="20">
         <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG11" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH11" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
-      </c>
+        <v>1.3</v>
+      </c>
+      <c r="AR11" s="2"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B12" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C12),MONTH(C12),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B12" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C12),MONTH(C12),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A12,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D12" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A12+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="2">
-        <v>20147130202</v>
+        <v>30707354719</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B12,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>60</v>
+      </c>
+      <c r="L12" s="1" t="e">
+        <f t="shared" ca="1" si="20"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M12" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N12" s="2">
-        <v>8851.52</v>
+        <v>1.2105263157894737</v>
+      </c>
+      <c r="N12" s="5">
+        <v>19000</v>
       </c>
       <c r="O12" s="5">
-        <v>9090.91</v>
+        <f t="shared" si="13"/>
+        <v>23000</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>38</v>
@@ -2434,286 +2919,408 @@
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="14">
+        <f>COUNTIFS($F$1:F12,F12,$K$1:K12,K12)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.210526</v>
+      </c>
+      <c r="W12" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X12" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V12" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y12" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W12" s="1" t="str">
+      <c r="Z12" s="1" t="str">
+        <f>TEXT(T12,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA12" s="13">
+        <f t="shared" si="3"/>
+        <v>3991.74</v>
+      </c>
+      <c r="AB12" s="13">
+        <f t="shared" si="15"/>
+        <v>23000</v>
+      </c>
+      <c r="AC12" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X12" s="14">
-        <f t="shared" si="14"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y12" s="14">
-        <f t="shared" si="15"/>
-        <v>11000</v>
-      </c>
-      <c r="Z12" s="10" t="str">
+        <v>23000.00</v>
+      </c>
+      <c r="AD12" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.00</v>
+      </c>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="AG12" s="15" t="str">
+        <f>J12&amp;"-"&amp;COUNTIF($J$1:J12,J12)</f>
+        <v>30707354719-1</v>
+      </c>
+      <c r="AH12" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI12" s="1">
         <f t="shared" si="7"/>
-        <v>9090.91</v>
-      </c>
-      <c r="AA12" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>B</v>
+      </c>
+      <c r="AK12" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="13">
         <f t="shared" si="17"/>
-        <v>12</v>
-      </c>
-      <c r="AD12" s="1" t="str">
-        <f>J12&amp;"-"&amp;COUNTIF($J$1:J12,J12)</f>
-        <v>20147130202-1</v>
-      </c>
-      <c r="AF12" s="15">
+        <v>23000</v>
+      </c>
+      <c r="AN12" s="13">
+        <f t="shared" si="9"/>
+        <v>19008.259999999998</v>
+      </c>
+      <c r="AO12" s="20">
+        <f t="shared" si="10"/>
+        <v>1.2105263157894737</v>
+      </c>
+      <c r="AP12" s="13">
+        <f t="shared" si="11"/>
+        <v>23000</v>
+      </c>
+      <c r="AQ12" s="20">
         <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG12" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH12" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
-      </c>
+        <v>1.2105263157894737</v>
+      </c>
+      <c r="AR12" s="2"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B13" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C13),MONTH(C13),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B13" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C13),MONTH(C13),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A13,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D13" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A13+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="2">
-        <v>30707354719</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L13" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B13,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>70</v>
+      </c>
+      <c r="L13" s="1" t="e">
+        <f t="shared" ca="1" si="20"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M13" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N13" s="2">
-        <v>8851.52</v>
+        <v>1.5</v>
+      </c>
+      <c r="N13" s="5">
+        <v>19000</v>
       </c>
       <c r="O13" s="5">
-        <v>9090.91</v>
-      </c>
-      <c r="P13" s="11" t="s">
-        <v>38</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>28500</v>
+      </c>
+      <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="14">
+        <f>COUNTIFS($F$1:F13,F13,$K$1:K13,K13)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W13" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X13" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="V13" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y13" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="W13" s="1" t="str">
+      <c r="Z13" s="1" t="str">
+        <f>TEXT(T13,"DD/MM/YYYY")</f>
+        <v>00/01/YYYY</v>
+      </c>
+      <c r="AA13" s="13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="13">
+        <f t="shared" si="15"/>
+        <v>28500</v>
+      </c>
+      <c r="AC13" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X13" s="14">
-        <f t="shared" si="14"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y13" s="14">
-        <f t="shared" si="15"/>
-        <v>11000</v>
-      </c>
-      <c r="Z13" s="10" t="str">
+        <v>28500.00</v>
+      </c>
+      <c r="AD13" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.00</v>
+      </c>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="AG13" s="15" t="str">
+        <f>J13&amp;"-"&amp;COUNTIF($J$1:J13,J13)</f>
+        <v>-0</v>
+      </c>
+      <c r="AH13" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI13" s="1">
         <f t="shared" si="7"/>
-        <v>11000.00</v>
-      </c>
-      <c r="AA13" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>C</v>
+      </c>
+      <c r="AK13" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="13">
         <f t="shared" si="17"/>
-        <v>13</v>
-      </c>
-      <c r="AD13" s="1" t="str">
-        <f>J13&amp;"-"&amp;COUNTIF($J$1:J13,J13)</f>
-        <v>30707354719-1</v>
-      </c>
-      <c r="AF13" s="15">
+        <v>28500</v>
+      </c>
+      <c r="AN13" s="13">
+        <f t="shared" si="9"/>
+        <v>28500</v>
+      </c>
+      <c r="AO13" s="20">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="AP13" s="13">
+        <f t="shared" si="11"/>
+        <v>28500</v>
+      </c>
+      <c r="AQ13" s="20">
         <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG13" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH13" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="AR13" s="2"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B14" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C14),MONTH(C14),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B14" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C14),MONTH(C14),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A14,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D14" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A14+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="2">
-        <v>37473042</v>
+        <v>9</v>
+      </c>
+      <c r="J14" s="3">
+        <v>30684125792</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L14" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B14,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>44</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="M14" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N14" s="2">
-        <v>8851.52</v>
+        <v>7.0247929999999998</v>
+      </c>
+      <c r="N14" s="5">
+        <v>19000</v>
       </c>
       <c r="O14" s="5">
-        <v>9090.91</v>
+        <f t="shared" si="13"/>
+        <v>133471.06700000001</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>00000</v>
-      </c>
-      <c r="V14" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>00000000</v>
-      </c>
-      <c r="W14" s="1" t="str">
+      <c r="Q14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T14" s="12">
+        <v>44816</v>
+      </c>
+      <c r="U14" s="14">
+        <f>COUNTIFS($F$1:F14,F14,$K$1:K14,K14)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>7.024793</v>
+      </c>
+      <c r="W14" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000150</v>
+      </c>
+      <c r="Z14" s="1" t="str">
+        <f>TEXT(T14,"DD/MM/YYYY")</f>
+        <v>12/09/YYYY</v>
+      </c>
+      <c r="AA14" s="13">
+        <f t="shared" si="3"/>
+        <v>28028.92</v>
+      </c>
+      <c r="AB14" s="13">
+        <f t="shared" si="15"/>
+        <v>161499.99</v>
+      </c>
+      <c r="AC14" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X14" s="14">
-        <f t="shared" si="14"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y14" s="14">
-        <f t="shared" si="15"/>
-        <v>11000</v>
-      </c>
-      <c r="Z14" s="10" t="str">
+        <v>133471.07</v>
+      </c>
+      <c r="AD14" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.01</v>
+      </c>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="AG14" s="15" t="str">
+        <f>J14&amp;"-"&amp;COUNTIF($J$1:J14,J14)</f>
+        <v>30684125792-1</v>
+      </c>
+      <c r="AH14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="1">
         <f t="shared" si="7"/>
-        <v>11000.00</v>
-      </c>
-      <c r="AA14" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK14" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="13">
         <f t="shared" si="17"/>
-        <v>14</v>
-      </c>
-      <c r="AD14" s="1" t="str">
-        <f>J14&amp;"-"&amp;COUNTIF($J$1:J14,J14)</f>
-        <v>37473042-1</v>
-      </c>
-      <c r="AF14" s="15">
+        <v>161499.99</v>
+      </c>
+      <c r="AN14" s="13">
+        <f t="shared" si="9"/>
+        <v>133471.07</v>
+      </c>
+      <c r="AO14" s="20">
+        <f t="shared" si="10"/>
+        <v>7.0247929999999998</v>
+      </c>
+      <c r="AP14" s="13">
+        <f t="shared" si="11"/>
+        <v>161500</v>
+      </c>
+      <c r="AQ14" s="20">
         <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG14" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH14" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
-      </c>
+        <v>7.0247929999999998</v>
+      </c>
+      <c r="AR14" s="2"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B15" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C15),MONTH(C15),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B15" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C15),MONTH(C15),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A15,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D15" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A15+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -2740,13 +3347,14 @@
         <v>64</v>
       </c>
       <c r="M15" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N15" s="2">
-        <v>8851.52</v>
+        <v>1.5</v>
+      </c>
+      <c r="N15" s="5">
+        <v>19000</v>
       </c>
       <c r="O15" s="5">
-        <v>9090.91</v>
+        <f t="shared" si="13"/>
+        <v>28500</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>38</v>
@@ -2760,194 +3368,273 @@
       <c r="S15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="T15" s="13">
+      <c r="T15" s="12">
         <v>44816</v>
       </c>
-      <c r="U15" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="U15" s="14">
+        <f>COUNTIFS($F$1:F15,F15,$K$1:K15,K15)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W15" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X15" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00002</v>
       </c>
-      <c r="V15" s="1" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y15" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000152</v>
       </c>
-      <c r="W15" s="1" t="str">
+      <c r="Z15" s="1" t="str">
+        <f>TEXT(T15,"DD/MM/YYYY")</f>
+        <v>12/09/YYYY</v>
+      </c>
+      <c r="AA15" s="13">
+        <f t="shared" si="3"/>
+        <v>4946.28</v>
+      </c>
+      <c r="AB15" s="13">
+        <f t="shared" si="15"/>
+        <v>28500</v>
+      </c>
+      <c r="AC15" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="X15" s="14">
-        <f t="shared" si="14"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y15" s="14">
-        <f t="shared" si="15"/>
-        <v>11000</v>
-      </c>
-      <c r="Z15" s="10" t="str">
-        <f t="shared" si="7"/>
-        <v>11000.00</v>
-      </c>
-      <c r="AA15" s="10" t="str">
-        <f t="shared" si="16"/>
+        <v>28500.00</v>
+      </c>
+      <c r="AD15" s="10" t="str">
+        <f t="shared" si="19"/>
         <v>0.00</v>
       </c>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1">
-        <f t="shared" si="17"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1">
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="AD15" s="1" t="str">
+      <c r="AG15" s="15" t="str">
         <f>J15&amp;"-"&amp;COUNTIF($J$1:J15,J15)</f>
         <v>30707354719-2</v>
       </c>
-      <c r="AF15" s="15">
+      <c r="AH15" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI15" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>B</v>
+      </c>
+      <c r="AK15" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="13">
+        <f t="shared" si="17"/>
+        <v>28500</v>
+      </c>
+      <c r="AN15" s="13">
+        <f t="shared" si="9"/>
+        <v>23553.72</v>
+      </c>
+      <c r="AO15" s="20">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="AP15" s="13">
+        <f t="shared" si="11"/>
+        <v>28500</v>
+      </c>
+      <c r="AQ15" s="20">
         <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG15" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH15" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="AR15" s="2"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B16" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C16),MONTH(C16),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B16" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C16),MONTH(C16),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A16,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D16" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A16+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" s="2">
-        <v>37473042</v>
+        <v>9</v>
+      </c>
+      <c r="J16" s="3">
+        <v>30684125792</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="M16" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N16" s="2">
-        <v>8851.52</v>
+        <v>7.003044</v>
+      </c>
+      <c r="N16" s="5">
+        <v>19000</v>
       </c>
       <c r="O16" s="5">
-        <v>9090.91</v>
+        <f t="shared" si="13"/>
+        <v>133057.83600000001</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>38</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="R16" s="11" t="s">
         <v>46</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="T16" s="13">
+        <v>49</v>
+      </c>
+      <c r="T16" s="12">
         <v>44816</v>
       </c>
-      <c r="U16" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="U16" s="14">
+        <f>COUNTIFS($F$1:F16,F16,$K$1:K16,K16)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V16" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>7.003044</v>
+      </c>
+      <c r="W16" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X16" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>00002</v>
       </c>
-      <c r="V16" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>00000153</v>
-      </c>
-      <c r="W16" s="1" t="str">
+      <c r="Y16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000151</v>
+      </c>
+      <c r="Z16" s="1" t="str">
+        <f>TEXT(T16,"DD/MM/YYYY")</f>
+        <v>12/09/YYYY</v>
+      </c>
+      <c r="AA16" s="13">
+        <f t="shared" si="3"/>
+        <v>27942.15</v>
+      </c>
+      <c r="AB16" s="13">
+        <f t="shared" si="15"/>
+        <v>160999.99</v>
+      </c>
+      <c r="AC16" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="X16" s="14">
-        <f t="shared" si="14"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y16" s="14">
-        <f t="shared" si="15"/>
-        <v>11000</v>
-      </c>
-      <c r="Z16" s="10" t="str">
+        <v>133057.84</v>
+      </c>
+      <c r="AD16" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.01</v>
+      </c>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="AG16" s="15" t="str">
+        <f>J16&amp;"-"&amp;COUNTIF($J$1:J16,J16)</f>
+        <v>30684125792-2</v>
+      </c>
+      <c r="AH16" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="1">
         <f t="shared" si="7"/>
-        <v>11000.00</v>
-      </c>
-      <c r="AA16" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AK16" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="13">
         <f t="shared" si="17"/>
-        <v>16</v>
-      </c>
-      <c r="AD16" s="1" t="str">
-        <f>J16&amp;"-"&amp;COUNTIF($J$1:J16,J16)</f>
-        <v>37473042-2</v>
-      </c>
-      <c r="AF16" s="15">
+        <v>160999.98000000001</v>
+      </c>
+      <c r="AN16" s="13">
+        <f t="shared" si="9"/>
+        <v>133057.82999999999</v>
+      </c>
+      <c r="AO16" s="20">
+        <f t="shared" si="10"/>
+        <v>7.003044</v>
+      </c>
+      <c r="AP16" s="13">
+        <f t="shared" si="11"/>
+        <v>161000</v>
+      </c>
+      <c r="AQ16" s="20">
         <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG16" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH16" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
-      </c>
+        <v>7.003044</v>
+      </c>
+      <c r="AR16" s="2"/>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>44992</v>
-      </c>
-      <c r="B17" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C17),MONTH(C17),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45069</v>
+      </c>
+      <c r="B17" s="9" t="e">
+        <f ca="1">TEXT(DATE(YEAR(C17),MONTH(C17),1),"dd/mm/YYYY")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>28/02/2023</v>
+        <f ca="1">TEXT(EOMONTH(A17,-1),"dd/mm/YYYY")</f>
+        <v>30/04/YYYY</v>
       </c>
       <c r="D17" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>21/03/2023</v>
+        <f ca="1">TEXT(A17+14,"dd/mm/YYYY")</f>
+        <v>06/06/YYYY</v>
       </c>
       <c r="E17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>39</v>
@@ -2958,86 +3645,134 @@
       <c r="I17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="2"/>
+      <c r="J17" s="2">
+        <v>37473042</v>
+      </c>
       <c r="K17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L17" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B17,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>56</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="M17" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N17" s="2">
-        <v>8851.52</v>
+        <v>1.5</v>
+      </c>
+      <c r="N17" s="5">
+        <v>19000</v>
       </c>
       <c r="O17" s="5">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>28500</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>00000</v>
-      </c>
-      <c r="V17" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>00000000</v>
-      </c>
-      <c r="W17" s="1" t="str">
+      <c r="Q17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="T17" s="12">
+        <v>44816</v>
+      </c>
+      <c r="U17" s="14">
+        <f>COUNTIFS($F$1:F17,F17,$K$1:K17,K17)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V17" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W17" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000153</v>
+      </c>
+      <c r="Z17" s="1" t="str">
+        <f>TEXT(T17,"DD/MM/YYYY")</f>
+        <v>12/09/YYYY</v>
+      </c>
+      <c r="AA17" s="13">
+        <f t="shared" si="3"/>
+        <v>4946.28</v>
+      </c>
+      <c r="AB17" s="13">
+        <f t="shared" si="15"/>
+        <v>28500</v>
+      </c>
+      <c r="AC17" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X17" s="14">
-        <f t="shared" si="14"/>
+        <v>28500.00</v>
+      </c>
+      <c r="AD17" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v>0.00</v>
+      </c>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="AG17" s="15" t="str">
+        <f>J17&amp;"-"&amp;COUNTIF($J$1:J17,J17)</f>
+        <v>37473042-2</v>
+      </c>
+      <c r="AH17" s="1">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y17" s="14">
-        <f t="shared" si="15"/>
+      <c r="AI17" s="1">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Z17" s="10" t="str">
-        <f>IF(F17="Factura A",SUBSTITUTE(TEXT(O17,"0,00"),",","."),SUBSTITUTE(TEXT(Y17,"0,00"),",","."))</f>
-        <v>0.00</v>
-      </c>
-      <c r="AA17" s="10" t="str">
+      <c r="AJ17" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>B</v>
+      </c>
+      <c r="AK17" s="1">
         <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="13">
         <f t="shared" si="17"/>
-        <v>17</v>
-      </c>
-      <c r="AD17" s="1" t="str">
-        <f>J17&amp;"-"&amp;COUNTIF($J$1:J17,J17)</f>
-        <v>-0</v>
-      </c>
-      <c r="AF17" s="15">
+        <v>28500</v>
+      </c>
+      <c r="AN17" s="13">
+        <f t="shared" si="9"/>
+        <v>23553.72</v>
+      </c>
+      <c r="AO17" s="20">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="AP17" s="13">
+        <f t="shared" si="11"/>
+        <v>28500</v>
+      </c>
+      <c r="AQ17" s="20">
         <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG17" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH17" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="AR17" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AB13">
-    <sortCondition ref="F2:F13"/>
-    <sortCondition ref="H2:H13"/>
-    <sortCondition ref="J2:J13"/>
+  <autoFilter ref="A1:AP17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO17">
+    <sortCondition ref="F2:F17"/>
+    <sortCondition ref="H2:H17"/>
+    <sortCondition ref="J2:J17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>